<commit_message>
Updated some stored procedures to add the Employee Type attribute when creating Invitation or OrgUser. Also updated ImportService and UserImportTemplate.xlsx file to add this attribute.
</commit_message>
<xml_diff>
--- a/AllyisApps/Resources/Files/UserImportTemplate.xlsx
+++ b/AllyisApps/Resources/Files/UserImportTemplate.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-jampo\Documents\AllyisApps\src\main\AllyisApps\Resources\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user1\Documents\AllyisApps\AllyisApps\AllyisApps\Resources\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About Importing" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>United States</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t xml:space="preserve">     The next sheet ("Users") demonstrates how to import users in bulk. Required columns have bold column headers in this example (you don't need to use bold for importing), and optional column headers are not bold. It is important that you spell the columns headers exactly as you see them here, but it does not matter what order the columns are in or if there are additional columns with other headers (they will be ignored). You may have empty cells in any of the non-required columns, but leaving out any of the information in the (bold) required columns will result in an error and a failure to import that user.</t>
+  </si>
+  <si>
+    <t>Employee Type</t>
+  </si>
+  <si>
+    <t>Salaried</t>
+  </si>
+  <si>
+    <t>Hourly</t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1037,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,18 +1057,20 @@
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1072,35 +1083,38 @@
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
@@ -1114,34 +1128,37 @@
         <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="6">
+      <c r="G2" s="6">
         <v>27660</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1155,34 +1172,37 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>30682</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>0</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="7">
+      <c r="L3" s="7">
         <v>12345</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1196,30 +1216,33 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>29038</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>25</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="7">
+      <c r="L4" s="7">
         <v>23456</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>26</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1232,7 +1255,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
   <ignoredErrors>
-    <ignoredError sqref="K2" numberStoredAsText="1"/>
+    <ignoredError sqref="L2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>